<commit_message>
Measured Times for 4096x4096 added
</commit_message>
<xml_diff>
--- a/PCP_-_#3_MPI_OpenMP_HybridSolution_Sparse_Matrix/resultados_Hibrido_2NODES_3MatricesSizes.xlsx
+++ b/PCP_-_#3_MPI_OpenMP_HybridSolution_Sparse_Matrix/resultados_Hibrido_2NODES_3MatricesSizes.xlsx
@@ -5103,7 +5103,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5433,7 +5433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AT598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L83" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O67" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>

</xml_diff>